<commit_message>
Updated with Message field tab.
</commit_message>
<xml_diff>
--- a/Subgroups/ASX/Extension Definition Exercises/ASX Sample Initialization Messages.xlsx
+++ b/Subgroups/ASX/Extension Definition Exercises/ASX Sample Initialization Messages.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosang\Documents\6 - SISO\C2SIMDocs\ASX\C2SIMArtifacts\Subgroups\ASX\Extension Definition Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11CB24-B3C7-4697-BF65-56F2EC37E46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A41F9-A2A4-460E-AB67-8537D991CC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{315F412D-A997-402A-95E2-E68C4026AE2E}"/>
+    <workbookView xWindow="1824" yWindow="3888" windowWidth="17280" windowHeight="8880" xr2:uid="{315F412D-A997-402A-95E2-E68C4026AE2E}"/>
   </bookViews>
   <sheets>
-    <sheet name="UAV with Video Init" sheetId="1" r:id="rId1"/>
-    <sheet name="UAV Patrol Initialization" sheetId="2" r:id="rId2"/>
-    <sheet name="Swarm Initialization" sheetId="3" r:id="rId3"/>
+    <sheet name="Initialization MessageBody Fiel" sheetId="4" r:id="rId1"/>
+    <sheet name="UAV with Video Init" sheetId="1" r:id="rId2"/>
+    <sheet name="UAV Patrol Initialization" sheetId="2" r:id="rId3"/>
+    <sheet name="Swarm Initialization" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>C2SIM Object</t>
   </si>
@@ -59,13 +60,148 @@
   </si>
   <si>
     <t>Parent Type</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Class that Defines Field</t>
+  </si>
+  <si>
+    <t>Model that defines attribute</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Root Element</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>C2SIM</t>
+  </si>
+  <si>
+    <t>See hasC2SIMHeader</t>
+  </si>
+  <si>
+    <t>hasC2SIMHeader</t>
+  </si>
+  <si>
+    <t>C2SIMHeader</t>
+  </si>
+  <si>
+    <t>SeeMessageBody</t>
+  </si>
+  <si>
+    <t>hasMessageBody</t>
+  </si>
+  <si>
+    <t>hasCommunicativeActTypeCode</t>
+  </si>
+  <si>
+    <t>CommunicativeActTypeCode</t>
+  </si>
+  <si>
+    <t>See JC3IEDM</t>
+  </si>
+  <si>
+    <t>hasSecurityClassificationCode</t>
+  </si>
+  <si>
+    <t>SecurityClassificationCode</t>
+  </si>
+  <si>
+    <t>hasSendingTime</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>hasProtocol</t>
+  </si>
+  <si>
+    <t>(hardcoded)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SISO-STD-C2SIM </t>
+  </si>
+  <si>
+    <t>hasProtocolVersion</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>See C2SIM Object Below</t>
+  </si>
+  <si>
+    <t>hasConversationId</t>
+  </si>
+  <si>
+    <t>UUIDBase</t>
+  </si>
+  <si>
+    <t>hasMessageId</t>
+  </si>
+  <si>
+    <t>isFromSendingSystem</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>isToReceivingSystem</t>
+  </si>
+  <si>
+    <t>hasReplyToSystem</t>
+  </si>
+  <si>
+    <t>isReplyToMessageId</t>
+  </si>
+  <si>
+    <t>C2SIMInitializationBody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hasInitializationFile </t>
+  </si>
+  <si>
+    <t>InitializationDataFile</t>
+  </si>
+  <si>
+    <t>hasObjectDefinitions</t>
+  </si>
+  <si>
+    <t>ObjectDefinitions</t>
+  </si>
+  <si>
+    <t>hasSystemEntityList</t>
+  </si>
+  <si>
+    <t>SystemEntityList</t>
+  </si>
+  <si>
+    <t>hasScenarioSetting</t>
+  </si>
+  <si>
+    <t>ScenarioSetting</t>
+  </si>
+  <si>
+    <t>hasTask</t>
+  </si>
+  <si>
+    <t>This varies for individual use cases.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +217,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,12 +266,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -448,6 +625,332 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18DA4BD-65F5-4B7D-9E28-58B65E4324DE}">
+  <dimension ref="A1:G68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A8839B-7B04-4264-BEF5-B002CE54D11F}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -490,7 +993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A8E33F-C1AB-4721-ABD8-DAB6B9B4CB63}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -533,11 +1036,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41331979-9D39-4390-90C7-8E12A1C4FBDD}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>

</xml_diff>